<commit_message>
cambio en el nombre
</commit_message>
<xml_diff>
--- a/diccionario veterinaria.xlsx
+++ b/diccionario veterinaria.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA\Documents\fredo\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D4750C4-A1C1-4757-A3F4-A773C6E8289A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BD9489-9126-4BD8-AC47-CD701A794E1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{395F164D-A499-42A4-AB21-A1DCA6D19906}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8880" xr2:uid="{395F164D-A499-42A4-AB21-A1DCA6D19906}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -217,37 +216,6 @@
     <t>Telefono del usuario.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Amasis MT Pro Black"/>
-        <family val="1"/>
-      </rPr>
-      <t>DICCIONARIO</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Amasis MT Pro Black"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Amasis MT Pro Black"/>
-        <family val="1"/>
-      </rPr>
-      <t>"CANES Y AMIGOS"</t>
-    </r>
-  </si>
-  <si>
     <t>CANES Y AMIGOS.</t>
   </si>
   <si>
@@ -408,6 +376,9 @@
   </si>
   <si>
     <t>COD_USU_MASC</t>
+  </si>
+  <si>
+    <t>la vete del fredo</t>
   </si>
 </sst>
 </file>
@@ -493,7 +464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -512,13 +483,16 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -981,63 +955,63 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD6AAB60-291B-4BB0-ABCA-C5E2D23FB0B5}">
   <dimension ref="A4:K89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="G69" sqref="G69"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" customWidth="1"/>
-    <col min="6" max="6" width="46.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" customWidth="1"/>
+    <col min="6" max="6" width="46.44140625" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:11" ht="21.75" x14ac:dyDescent="0.4">
-      <c r="D4" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
+    <row r="4" spans="1:11" ht="21.6" x14ac:dyDescent="0.45">
+      <c r="D4" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
     </row>
-    <row r="8" spans="1:11" ht="22.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" ht="21" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:11" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" ht="18.600000000000001" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1060,12 +1034,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C11" t="s">
         <v>17</v>
@@ -1083,12 +1057,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
@@ -1103,10 +1077,10 @@
         <v>21</v>
       </c>
       <c r="G12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1129,12 +1103,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C14" t="s">
         <v>17</v>
@@ -1152,33 +1126,33 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="22.5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" ht="21" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-    </row>
-    <row r="18" spans="1:7" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+    </row>
+    <row r="18" spans="1:7" ht="18.600000000000001" x14ac:dyDescent="0.45">
       <c r="A18" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -1201,7 +1175,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -1224,12 +1198,12 @@
         <v>1017213938</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C21" t="s">
         <v>17</v>
@@ -1247,7 +1221,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -1270,12 +1244,12 @@
         <v>3003704921</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>34</v>
       </c>
       <c r="B23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C23" t="s">
         <v>17</v>
@@ -1293,33 +1267,33 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="22.5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" ht="21" x14ac:dyDescent="0.5">
       <c r="A26" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-    </row>
-    <row r="27" spans="1:7" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+    </row>
+    <row r="27" spans="1:7" ht="18.600000000000001" x14ac:dyDescent="0.45">
       <c r="A27" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -1342,7 +1316,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -1365,12 +1339,12 @@
         <v>43664388</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C30" t="s">
         <v>17</v>
@@ -1388,7 +1362,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -1411,12 +1385,12 @@
         <v>3103203456</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>45</v>
       </c>
       <c r="B32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C32" t="s">
         <v>17</v>
@@ -1434,33 +1408,33 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="22.5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" ht="21" x14ac:dyDescent="0.5">
       <c r="A35" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-    </row>
-    <row r="36" spans="1:7" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+    </row>
+    <row r="36" spans="1:7" ht="18.600000000000001" x14ac:dyDescent="0.45">
       <c r="A36" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -1483,76 +1457,76 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B38" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F38" t="s">
         <v>80</v>
-      </c>
-      <c r="C38" t="s">
-        <v>17</v>
-      </c>
-      <c r="D38" t="s">
-        <v>17</v>
-      </c>
-      <c r="E38" t="s">
-        <v>17</v>
-      </c>
-      <c r="F38" t="s">
-        <v>81</v>
       </c>
       <c r="G38" s="7">
         <v>44868</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B39" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39" t="s">
+        <v>17</v>
+      </c>
+      <c r="F39" t="s">
+        <v>81</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>78</v>
       </c>
-      <c r="C39" t="s">
-        <v>17</v>
-      </c>
-      <c r="D39" t="s">
-        <v>17</v>
-      </c>
-      <c r="E39" t="s">
-        <v>17</v>
-      </c>
-      <c r="F39" t="s">
+      <c r="B40" t="s">
+        <v>77</v>
+      </c>
+      <c r="C40" t="s">
+        <v>17</v>
+      </c>
+      <c r="D40" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40" t="s">
+        <v>17</v>
+      </c>
+      <c r="F40" t="s">
         <v>82</v>
       </c>
-      <c r="G39" s="6" t="s">
+      <c r="G40" s="6" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>79</v>
-      </c>
-      <c r="B40" t="s">
-        <v>78</v>
-      </c>
-      <c r="C40" t="s">
-        <v>17</v>
-      </c>
-      <c r="D40" t="s">
-        <v>17</v>
-      </c>
-      <c r="E40" t="s">
-        <v>17</v>
-      </c>
-      <c r="F40" t="s">
-        <v>83</v>
-      </c>
-      <c r="G40" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>49</v>
       </c>
@@ -1575,7 +1549,7 @@
         <v>43664388</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>50</v>
       </c>
@@ -1598,33 +1572,33 @@
         <v>1017213938</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="22.5" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" ht="21" x14ac:dyDescent="0.5">
       <c r="A45" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B45" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
-    </row>
-    <row r="46" spans="1:7" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+    </row>
+    <row r="46" spans="1:7" ht="18.600000000000001" x14ac:dyDescent="0.45">
       <c r="A46" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="B46" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>4</v>
       </c>
@@ -1647,7 +1621,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>53</v>
       </c>
@@ -1670,12 +1644,12 @@
         <v>10132553444</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>57</v>
       </c>
       <c r="B49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C49" t="s">
         <v>17</v>
@@ -1693,7 +1667,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>58</v>
       </c>
@@ -1716,12 +1690,12 @@
         <v>3145463467</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B51" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C51" t="s">
         <v>17</v>
@@ -1739,33 +1713,33 @@
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="22.5" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:7" ht="21" x14ac:dyDescent="0.5">
       <c r="A54" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B54" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="8"/>
-      <c r="F54" s="8"/>
-      <c r="G54" s="8"/>
-    </row>
-    <row r="55" spans="1:7" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B54" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="9"/>
+    </row>
+    <row r="55" spans="1:7" ht="18.600000000000001" x14ac:dyDescent="0.45">
       <c r="A55" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B55" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="C55" s="9"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="9"/>
-      <c r="F55" s="9"/>
-      <c r="G55" s="9"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B55" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="10"/>
+      <c r="G55" s="10"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>4</v>
       </c>
@@ -1788,9 +1762,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B57" t="s">
         <v>16</v>
@@ -1805,18 +1779,18 @@
         <v>17</v>
       </c>
       <c r="F57" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G57" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B58" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C58" t="s">
         <v>17</v>
@@ -1828,15 +1802,15 @@
         <v>17</v>
       </c>
       <c r="F58" t="s">
+        <v>101</v>
+      </c>
+      <c r="G58" t="s">
         <v>102</v>
       </c>
-      <c r="G58" t="s">
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>104</v>
       </c>
       <c r="B59" t="s">
         <v>16</v>
@@ -1857,12 +1831,12 @@
         <v>1017213938</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B60" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C60" t="s">
         <v>17</v>
@@ -1880,33 +1854,33 @@
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="22.5" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:7" ht="21" x14ac:dyDescent="0.5">
       <c r="A63" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B63" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="C63" s="8"/>
-      <c r="D63" s="8"/>
-      <c r="E63" s="8"/>
-      <c r="F63" s="8"/>
-      <c r="G63" s="8"/>
-    </row>
-    <row r="64" spans="1:7" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B63" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="9"/>
+      <c r="G63" s="9"/>
+    </row>
+    <row r="64" spans="1:7" ht="18.600000000000001" x14ac:dyDescent="0.45">
       <c r="A64" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B64" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C64" s="9"/>
-      <c r="D64" s="9"/>
-      <c r="E64" s="9"/>
-      <c r="F64" s="9"/>
-      <c r="G64" s="9"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B64" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="10"/>
+      <c r="F64" s="10"/>
+      <c r="G64" s="10"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>4</v>
       </c>
@@ -1929,12 +1903,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B66" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C66" t="s">
         <v>17</v>
@@ -1946,18 +1920,18 @@
         <v>17</v>
       </c>
       <c r="F66" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G66" s="7">
         <v>44809</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B67" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C67" t="s">
         <v>17</v>
@@ -1969,15 +1943,15 @@
         <v>17</v>
       </c>
       <c r="F67" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G67" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B68" t="s">
         <v>16</v>
@@ -1998,9 +1972,9 @@
         <v>43664388</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B69" t="s">
         <v>16</v>
@@ -2021,9 +1995,9 @@
         <v>1017213938</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B70" t="s">
         <v>16</v>
@@ -2038,39 +2012,39 @@
         <v>18</v>
       </c>
       <c r="F70" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G70" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="22.5" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:7" ht="21" x14ac:dyDescent="0.5">
       <c r="A73" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B73" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C73" s="8"/>
-      <c r="D73" s="8"/>
-      <c r="E73" s="8"/>
-      <c r="F73" s="8"/>
-      <c r="G73" s="8"/>
-    </row>
-    <row r="74" spans="1:7" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B73" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C73" s="9"/>
+      <c r="D73" s="9"/>
+      <c r="E73" s="9"/>
+      <c r="F73" s="9"/>
+      <c r="G73" s="9"/>
+    </row>
+    <row r="74" spans="1:7" ht="18.600000000000001" x14ac:dyDescent="0.45">
       <c r="A74" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B74" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="C74" s="9"/>
-      <c r="D74" s="9"/>
-      <c r="E74" s="9"/>
-      <c r="F74" s="9"/>
-      <c r="G74" s="9"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B74" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C74" s="10"/>
+      <c r="D74" s="10"/>
+      <c r="E74" s="10"/>
+      <c r="F74" s="10"/>
+      <c r="G74" s="10"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>4</v>
       </c>
@@ -2093,9 +2067,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B76" t="s">
         <v>16</v>
@@ -2110,15 +2084,15 @@
         <v>17</v>
       </c>
       <c r="F76" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G76" s="6">
         <v>34678</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B77" t="s">
         <v>16</v>
@@ -2133,15 +2107,15 @@
         <v>17</v>
       </c>
       <c r="F77" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G77" s="6">
         <v>5000</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B78" t="s">
         <v>15</v>
@@ -2156,15 +2130,15 @@
         <v>17</v>
       </c>
       <c r="F78" t="s">
+        <v>68</v>
+      </c>
+      <c r="G78" t="s">
         <v>69</v>
       </c>
-      <c r="G78" t="s">
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>71</v>
       </c>
       <c r="B79" t="s">
         <v>16</v>
@@ -2179,15 +2153,15 @@
         <v>17</v>
       </c>
       <c r="F79" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G79" s="6">
         <v>3145463467</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B80" t="s">
         <v>14</v>
@@ -2208,33 +2182,33 @@
         <v>20</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="22.5" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:7" ht="21" x14ac:dyDescent="0.5">
       <c r="A83" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B83" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C83" s="8"/>
-      <c r="D83" s="8"/>
-      <c r="E83" s="8"/>
-      <c r="F83" s="8"/>
-      <c r="G83" s="8"/>
-    </row>
-    <row r="84" spans="1:7" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B83" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C83" s="9"/>
+      <c r="D83" s="9"/>
+      <c r="E83" s="9"/>
+      <c r="F83" s="9"/>
+      <c r="G83" s="9"/>
+    </row>
+    <row r="84" spans="1:7" ht="18.600000000000001" x14ac:dyDescent="0.45">
       <c r="A84" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B84" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="C84" s="9"/>
-      <c r="D84" s="9"/>
-      <c r="E84" s="9"/>
-      <c r="F84" s="9"/>
-      <c r="G84" s="9"/>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B84" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C84" s="10"/>
+      <c r="D84" s="10"/>
+      <c r="E84" s="10"/>
+      <c r="F84" s="10"/>
+      <c r="G84" s="10"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>4</v>
       </c>
@@ -2257,9 +2231,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B86" t="s">
         <v>14</v>
@@ -2274,38 +2248,38 @@
         <v>17</v>
       </c>
       <c r="F86" t="s">
+        <v>108</v>
+      </c>
+      <c r="G86" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="G86" s="6" t="s">
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+      <c r="B87" t="s">
+        <v>86</v>
+      </c>
+      <c r="C87" t="s">
+        <v>17</v>
+      </c>
+      <c r="D87" t="s">
+        <v>17</v>
+      </c>
+      <c r="E87" t="s">
+        <v>17</v>
+      </c>
+      <c r="F87" t="s">
         <v>111</v>
       </c>
-      <c r="B87" t="s">
-        <v>87</v>
-      </c>
-      <c r="C87" t="s">
-        <v>17</v>
-      </c>
-      <c r="D87" t="s">
-        <v>17</v>
-      </c>
-      <c r="E87" t="s">
-        <v>17</v>
-      </c>
-      <c r="F87" t="s">
+      <c r="G87" t="s">
         <v>112</v>
       </c>
-      <c r="G87" t="s">
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>114</v>
       </c>
       <c r="B88" t="s">
         <v>16</v>
@@ -2326,12 +2300,12 @@
         <v>43664388</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B89" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C89" t="s">
         <v>17</v>
@@ -2351,6 +2325,10 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B83:G83"/>
+    <mergeCell ref="B84:G84"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="B73:G73"/>
     <mergeCell ref="B74:G74"/>
@@ -2366,10 +2344,6 @@
     <mergeCell ref="B36:G36"/>
     <mergeCell ref="B54:G54"/>
     <mergeCell ref="B55:G55"/>
-    <mergeCell ref="B83:G83"/>
-    <mergeCell ref="B84:G84"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>